<commit_message>
done until sturctural model
</commit_message>
<xml_diff>
--- a/Data/Data_geology/Otorowiri_Model_Geology.xlsx
+++ b/Data/Data_geology/Otorowiri_Model_Geology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105010\Projects\Otorowiri\data\data_geology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CA4B48-E1C2-4A8D-8DDB-1F4FD2254149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D77BE1-9AFF-4178-9516-2D70359845B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{F0865505-9651-490B-8489-90EAB7C11998}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F0865505-9651-490B-8489-90EAB7C11998}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
@@ -423,9 +423,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -463,7 +463,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -569,7 +569,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -711,7 +711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -722,7 +722,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3390,7 +3390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B9F143-9958-4935-B8DD-39F9BB800345}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3399,11 +3401,12 @@
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>42</v>
@@ -4952,9 +4955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3CA644-E985-404A-BE16-92C33830C9B0}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
updated based on Perth model. Geomodel working
</commit_message>
<xml_diff>
--- a/Data/Data_geology/Otorowiri_Model_Geology.xlsx
+++ b/Data/Data_geology/Otorowiri_Model_Geology.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105010\Projects\Otorowiri\data\data_geology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105295\Projects\Otorowiri\Data\Data_geology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA952B40-102B-48C5-9690-4382A37EC89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9BE01C-49C9-4FCE-BFB9-61FEBACB9E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="6" xr2:uid="{F0865505-9651-490B-8489-90EAB7C11998}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18430" windowHeight="11020" firstSheet="2" activeTab="2" xr2:uid="{F0865505-9651-490B-8489-90EAB7C11998}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="130">
   <si>
     <t>Dongara Line DL3A</t>
   </si>
@@ -422,6 +422,21 @@
   </si>
   <si>
     <t>Mapping Kpo outcrop</t>
+  </si>
+  <si>
+    <t>iconvert</t>
+  </si>
+  <si>
+    <t>hk</t>
+  </si>
+  <si>
+    <t>vk</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>sy</t>
   </si>
 </sst>
 </file>
@@ -534,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,6 +606,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +932,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="53.6328125" customWidth="1"/>
+    <col min="2" max="2" width="53.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1103,18 +1122,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4789AD-4A52-4EB4-A331-3432CA489414}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="9" max="13" width="9.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>94</v>
       </c>
@@ -1139,8 +1159,23 @@
       <c r="H1" s="13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>102</v>
       </c>
@@ -1165,8 +1200,9 @@
       <c r="H2" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>104</v>
       </c>
@@ -1192,8 +1228,23 @@
         <f>F2-F3</f>
         <v>175.74074074074073</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="22">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>104</v>
       </c>
@@ -1219,8 +1270,23 @@
         <f>F3-F4</f>
         <v>59.321759259259267</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.1</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>104</v>
       </c>
@@ -1246,8 +1312,23 @@
         <f t="shared" ref="H5:H14" si="0">F4-F5</f>
         <v>201.76358695652175</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>104</v>
       </c>
@@ -1273,8 +1354,23 @@
         <f t="shared" si="0"/>
         <v>383.17391304347825</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>104</v>
       </c>
@@ -1300,8 +1396,23 @@
         <f t="shared" si="0"/>
         <v>277.59999999999991</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>104</v>
       </c>
@@ -1327,8 +1438,23 @@
         <f t="shared" si="0"/>
         <v>585.73333333333335</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>104</v>
       </c>
@@ -1354,8 +1480,23 @@
         <f t="shared" si="0"/>
         <v>254.4666666666667</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+      <c r="L9" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>104</v>
       </c>
@@ -1381,8 +1522,23 @@
         <f t="shared" si="0"/>
         <v>490.20000000000005</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>104</v>
       </c>
@@ -1408,8 +1564,23 @@
         <f t="shared" si="0"/>
         <v>617</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M11">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>104</v>
       </c>
@@ -1435,8 +1606,23 @@
         <f t="shared" si="0"/>
         <v>357.66666666666652</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>104</v>
       </c>
@@ -1462,8 +1648,23 @@
         <f t="shared" si="0"/>
         <v>107.08333333333348</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>104</v>
       </c>
@@ -1489,6 +1690,45 @@
         <f t="shared" si="0"/>
         <v>368.75</v>
       </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" s="23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I15" s="6"/>
+      <c r="L15" s="23"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I16" s="6"/>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.35">
+      <c r="I17" s="6"/>
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.35">
+      <c r="I18" s="6"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="9:12" x14ac:dyDescent="0.35">
+      <c r="I19" s="6"/>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="9:12" x14ac:dyDescent="0.35">
+      <c r="I20" s="6"/>
+      <c r="L20" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1505,7 +1745,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
     <col min="2" max="2" width="8.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" customWidth="1"/>
@@ -3988,7 +4228,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
     <col min="2" max="2" width="8.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
@@ -5547,13 +5787,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED891851-15F7-4B61-A48B-7C8AA2AA41A2}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
     <col min="2" max="2" width="8.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
@@ -7019,8 +7259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3CA644-E985-404A-BE16-92C33830C9B0}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7108,7 +7348,8 @@
         <v>109</v>
       </c>
       <c r="F2" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A2,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>209</v>
       </c>
       <c r="G2" s="3">
         <v>167</v>
@@ -7134,7 +7375,8 @@
         <v>109</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A3,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>209</v>
       </c>
       <c r="G3" s="3">
         <v>167</v>
@@ -7160,7 +7402,8 @@
         <v>109</v>
       </c>
       <c r="F4" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A4,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>256</v>
       </c>
       <c r="G4" s="3">
         <v>102</v>
@@ -7183,7 +7426,8 @@
         <v>109</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A5,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>256</v>
       </c>
       <c r="G5" s="3">
         <v>102</v>
@@ -7206,7 +7450,8 @@
         <v>109</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A6,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>311</v>
       </c>
       <c r="G6" s="3">
         <v>107</v>
@@ -7238,7 +7483,8 @@
         <v>109</v>
       </c>
       <c r="F7" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A7,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>311</v>
       </c>
       <c r="G7" s="3">
         <v>107</v>
@@ -7268,7 +7514,8 @@
         <v>109</v>
       </c>
       <c r="F8" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A8,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>228</v>
       </c>
       <c r="G8" s="3">
         <v>107</v>
@@ -7291,7 +7538,8 @@
         <v>109</v>
       </c>
       <c r="F9" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A9,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>228</v>
       </c>
       <c r="G9" s="3">
         <v>107</v>
@@ -7314,7 +7562,8 @@
         <v>109</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A10,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>203</v>
       </c>
       <c r="H10" s="3">
         <v>31</v>
@@ -7343,7 +7592,8 @@
         <v>109</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A11,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>203</v>
       </c>
       <c r="G11" s="21">
         <v>0</v>
@@ -7373,7 +7623,8 @@
         <v>109</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A12,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>222</v>
       </c>
       <c r="G12" s="3">
         <v>137</v>
@@ -7396,7 +7647,8 @@
         <v>109</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A13,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>222</v>
       </c>
       <c r="G13" s="3">
         <v>137</v>
@@ -7419,7 +7671,8 @@
         <v>109</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A14,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>208</v>
       </c>
       <c r="G14" s="3">
         <v>183</v>
@@ -7442,7 +7695,8 @@
         <v>109</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A15,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>208</v>
       </c>
       <c r="G15" s="3">
         <v>183</v>
@@ -7465,7 +7719,8 @@
         <v>109</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A16,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>227</v>
       </c>
       <c r="G16" s="3">
         <v>195</v>
@@ -7488,7 +7743,8 @@
         <v>109</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A17,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>227</v>
       </c>
       <c r="G17" s="3">
         <v>195</v>
@@ -7511,7 +7767,8 @@
         <v>109</v>
       </c>
       <c r="F18" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A18,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>218</v>
       </c>
       <c r="G18" s="3">
         <v>152</v>
@@ -7534,7 +7791,8 @@
         <v>109</v>
       </c>
       <c r="F19" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A19,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>218</v>
       </c>
       <c r="G19" s="3">
         <v>152</v>
@@ -7557,7 +7815,8 @@
         <v>109</v>
       </c>
       <c r="F20" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A20,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>222</v>
       </c>
       <c r="G20" s="3">
         <v>110</v>
@@ -7580,7 +7839,8 @@
         <v>109</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A21,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>222</v>
       </c>
       <c r="G21" s="3">
         <v>110</v>
@@ -7603,7 +7863,8 @@
         <v>109</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A22,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>272</v>
       </c>
       <c r="G22" s="3">
         <v>195</v>
@@ -7629,7 +7890,8 @@
         <v>109</v>
       </c>
       <c r="F23" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A23,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>272</v>
       </c>
       <c r="G23" s="3">
         <v>195</v>
@@ -7655,7 +7917,8 @@
         <v>109</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A24,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>265</v>
       </c>
       <c r="G24" s="3">
         <v>247</v>
@@ -7678,7 +7941,8 @@
         <v>109</v>
       </c>
       <c r="F25" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A25,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>265</v>
       </c>
       <c r="G25" s="3">
         <v>247</v>
@@ -7701,7 +7965,8 @@
         <v>109</v>
       </c>
       <c r="F26" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A26,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>222</v>
       </c>
       <c r="H26" s="3">
         <v>67</v>
@@ -7730,7 +7995,8 @@
         <v>109</v>
       </c>
       <c r="F27" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A27,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>222</v>
       </c>
       <c r="G27" s="21">
         <v>0</v>
@@ -7760,7 +8026,8 @@
         <v>109</v>
       </c>
       <c r="F28" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A28,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>276</v>
       </c>
       <c r="G28" s="3">
         <v>94</v>
@@ -7792,7 +8059,8 @@
         <v>109</v>
       </c>
       <c r="F29" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A29,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>276</v>
       </c>
       <c r="G29" s="3">
         <v>94</v>
@@ -7822,7 +8090,8 @@
         <v>109</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A30,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>184</v>
       </c>
       <c r="I30" s="3">
         <v>241</v>
@@ -7848,7 +8117,8 @@
         <v>109</v>
       </c>
       <c r="F31" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A31,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>184</v>
       </c>
       <c r="G31" s="21">
         <v>0</v>
@@ -7878,7 +8148,8 @@
         <v>109</v>
       </c>
       <c r="F32" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A32,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>283</v>
       </c>
       <c r="G32" s="3">
         <v>183</v>
@@ -7910,7 +8181,8 @@
         <v>109</v>
       </c>
       <c r="F33" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A33,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>283</v>
       </c>
       <c r="G33" s="3">
         <v>183</v>
@@ -7940,7 +8212,8 @@
         <v>109</v>
       </c>
       <c r="F34" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A34,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>267</v>
       </c>
       <c r="G34" s="3">
         <v>159</v>
@@ -7972,7 +8245,8 @@
         <v>109</v>
       </c>
       <c r="F35" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A35,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>267</v>
       </c>
       <c r="G35" s="3">
         <v>159</v>
@@ -8002,7 +8276,8 @@
         <v>109</v>
       </c>
       <c r="F36" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A36,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>306</v>
       </c>
       <c r="G36" s="3">
         <v>204</v>
@@ -8028,7 +8303,8 @@
         <v>109</v>
       </c>
       <c r="F37" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A37,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>306</v>
       </c>
       <c r="G37" s="3">
         <v>204</v>
@@ -8055,7 +8331,8 @@
         <v>109</v>
       </c>
       <c r="F38" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A38,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>280</v>
       </c>
       <c r="G38" s="3">
         <v>302</v>
@@ -8078,7 +8355,8 @@
         <v>109</v>
       </c>
       <c r="F39" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A39,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>280</v>
       </c>
       <c r="G39" s="3">
         <v>302</v>
@@ -8101,7 +8379,8 @@
         <v>109</v>
       </c>
       <c r="F40" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A40,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>258</v>
       </c>
       <c r="G40" s="3">
         <v>85</v>
@@ -8133,7 +8412,8 @@
         <v>109</v>
       </c>
       <c r="F41" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A41,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>258</v>
       </c>
       <c r="G41" s="3">
         <v>85</v>
@@ -8163,7 +8443,8 @@
         <v>109</v>
       </c>
       <c r="F42" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A42,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>169</v>
       </c>
       <c r="I42" s="3">
         <v>221</v>
@@ -8189,7 +8470,8 @@
         <v>109</v>
       </c>
       <c r="F43" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A43,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>169</v>
       </c>
       <c r="G43" s="21">
         <v>0</v>
@@ -8219,7 +8501,8 @@
         <v>109</v>
       </c>
       <c r="F44" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A44,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>231</v>
       </c>
       <c r="G44" s="3">
         <v>158</v>
@@ -8242,7 +8525,8 @@
         <v>109</v>
       </c>
       <c r="F45" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A45,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>231</v>
       </c>
       <c r="G45" s="3">
         <v>158</v>
@@ -8266,7 +8550,8 @@
         <v>109</v>
       </c>
       <c r="F46" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A46,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>193</v>
       </c>
       <c r="I46" s="3">
         <v>200</v>
@@ -8292,7 +8577,8 @@
         <v>109</v>
       </c>
       <c r="F47" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A47,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>193</v>
       </c>
       <c r="G47" s="21">
         <v>0</v>
@@ -8322,7 +8608,8 @@
         <v>109</v>
       </c>
       <c r="F48" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A48,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>128</v>
       </c>
       <c r="I48" s="3">
         <v>484</v>
@@ -8348,7 +8635,8 @@
         <v>109</v>
       </c>
       <c r="F49" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A49,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>128</v>
       </c>
       <c r="G49" s="21">
         <v>0</v>
@@ -8378,7 +8666,8 @@
         <v>109</v>
       </c>
       <c r="F50" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A50,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>258</v>
       </c>
       <c r="G50" s="3">
         <v>25</v>
@@ -8410,7 +8699,8 @@
         <v>109</v>
       </c>
       <c r="F51" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A51,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>258</v>
       </c>
       <c r="G51" s="3">
         <v>25</v>
@@ -8440,7 +8730,8 @@
         <v>109</v>
       </c>
       <c r="F52" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A52,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>299</v>
       </c>
       <c r="G52" s="3">
         <v>199</v>
@@ -8472,7 +8763,8 @@
         <v>109</v>
       </c>
       <c r="F53" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A53,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>299</v>
       </c>
       <c r="G53" s="3">
         <v>199</v>
@@ -8502,7 +8794,8 @@
         <v>109</v>
       </c>
       <c r="F54" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A54,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>107</v>
       </c>
       <c r="I54" s="3">
         <v>220</v>
@@ -8555,7 +8848,8 @@
         <v>109</v>
       </c>
       <c r="F55" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A55,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>107</v>
       </c>
       <c r="G55" s="21">
         <v>0</v>
@@ -8612,7 +8906,8 @@
         <v>109</v>
       </c>
       <c r="F56" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A56,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>280</v>
       </c>
       <c r="G56" s="3">
         <v>70</v>
@@ -8635,7 +8930,8 @@
         <v>109</v>
       </c>
       <c r="F57" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A57,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>280</v>
       </c>
       <c r="G57" s="3">
         <v>70</v>
@@ -8658,7 +8954,8 @@
         <v>109</v>
       </c>
       <c r="F58" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A58,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>281</v>
       </c>
       <c r="G58" s="3">
         <v>105</v>
@@ -8681,7 +8978,8 @@
         <v>109</v>
       </c>
       <c r="F59" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A59,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>281</v>
       </c>
       <c r="G59" s="3">
         <v>105</v>
@@ -8704,7 +9002,8 @@
         <v>109</v>
       </c>
       <c r="F60" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A60,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>123</v>
       </c>
       <c r="I60" s="3">
         <v>324</v>
@@ -8757,7 +9056,8 @@
         <v>109</v>
       </c>
       <c r="F61" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A61,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>123</v>
       </c>
       <c r="G61" s="21">
         <v>0</v>
@@ -8814,7 +9114,8 @@
         <v>109</v>
       </c>
       <c r="F62" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A62,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>257</v>
       </c>
       <c r="G62" s="3">
         <v>291</v>
@@ -8846,7 +9147,8 @@
         <v>109</v>
       </c>
       <c r="F63" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A63,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>257</v>
       </c>
       <c r="G63" s="3">
         <v>291</v>
@@ -8876,7 +9178,8 @@
         <v>109</v>
       </c>
       <c r="F64" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A64,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>264</v>
       </c>
       <c r="G64" s="3">
         <v>378</v>
@@ -8908,7 +9211,8 @@
         <v>109</v>
       </c>
       <c r="F65" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A65,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>264</v>
       </c>
       <c r="G65" s="3">
         <v>378</v>
@@ -8938,7 +9242,8 @@
         <v>109</v>
       </c>
       <c r="F66" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A66,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>295</v>
       </c>
       <c r="G66" s="3">
         <v>434</v>
@@ -8970,7 +9275,8 @@
         <v>109</v>
       </c>
       <c r="F67" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A67,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>295</v>
       </c>
       <c r="G67" s="3">
         <v>434</v>
@@ -9000,7 +9306,8 @@
         <v>109</v>
       </c>
       <c r="F68" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A68,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>254</v>
       </c>
       <c r="G68" s="3">
         <v>216</v>
@@ -9032,7 +9339,8 @@
         <v>109</v>
       </c>
       <c r="F69" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A69,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>254</v>
       </c>
       <c r="G69" s="3">
         <v>216</v>
@@ -9062,7 +9370,8 @@
         <v>109</v>
       </c>
       <c r="F70" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A70,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>201</v>
       </c>
       <c r="I70" s="3">
         <v>716</v>
@@ -9088,7 +9397,8 @@
         <v>109</v>
       </c>
       <c r="F71" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A71,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>201</v>
       </c>
       <c r="G71" s="21">
         <v>0</v>
@@ -9118,7 +9428,8 @@
         <v>109</v>
       </c>
       <c r="F72" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A72,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>139</v>
       </c>
       <c r="K72" s="3">
         <v>418</v>
@@ -9147,7 +9458,8 @@
         <v>109</v>
       </c>
       <c r="F73" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A73,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>139</v>
       </c>
       <c r="G73" s="21">
         <v>0</v>
@@ -9186,7 +9498,8 @@
         <v>109</v>
       </c>
       <c r="F74" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A74,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>233</v>
       </c>
       <c r="I74" s="3">
         <v>800</v>
@@ -9233,7 +9546,8 @@
         <v>109</v>
       </c>
       <c r="F75" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A75,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>233</v>
       </c>
       <c r="I75" s="3">
         <v>800</v>
@@ -9278,7 +9592,8 @@
         <v>109</v>
       </c>
       <c r="F76" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A76,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>241</v>
       </c>
       <c r="L76" s="11">
         <v>2023</v>
@@ -9322,7 +9637,8 @@
         <v>109</v>
       </c>
       <c r="F77" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A77,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>241</v>
       </c>
       <c r="L77" s="16">
         <v>2023</v>
@@ -9364,7 +9680,8 @@
         <v>109</v>
       </c>
       <c r="F78" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A78,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>148</v>
       </c>
       <c r="I78" s="3">
         <v>340</v>
@@ -9390,7 +9707,8 @@
         <v>109</v>
       </c>
       <c r="F79" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A79,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>148</v>
       </c>
       <c r="G79" s="21">
         <v>0</v>
@@ -9420,7 +9738,8 @@
         <v>109</v>
       </c>
       <c r="F80" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A80,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>266</v>
       </c>
       <c r="G80" s="3">
         <v>140</v>
@@ -9443,7 +9762,8 @@
         <v>109</v>
       </c>
       <c r="F81" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A81,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>266</v>
       </c>
       <c r="G81" s="3">
         <v>140</v>
@@ -9467,7 +9787,8 @@
         <v>109</v>
       </c>
       <c r="F82" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A82,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>220</v>
       </c>
       <c r="I82" s="3">
         <v>600</v>
@@ -9505,7 +9826,8 @@
         <v>109</v>
       </c>
       <c r="F83" s="3">
-        <v>0</v>
+        <f>VLOOKUP(A83,mAHD!$A$2:$D$42,4,FALSE)</f>
+        <v>220</v>
       </c>
       <c r="G83" s="21">
         <v>0</v>
@@ -9809,7 +10131,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>